<commit_message>
feat: Fill readiness to icp store
</commit_message>
<xml_diff>
--- a/public/assets/file/Template_ICP.xlsx
+++ b/public/assets/file/Template_ICP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\core\public\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39F66A8-820C-4153-8AE7-97CF6D4B9CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD60CE94-AE85-42AC-B74C-D7D5B0EE355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
   <si>
     <t>INDIVIDUAL CAREER PLAN (ICP)</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t xml:space="preserve">Readiness </t>
-  </si>
-  <si>
-    <t>Year :</t>
   </si>
   <si>
     <t>Level / Sub-Level</t>
@@ -764,7 +761,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -890,181 +887,180 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1464,7 +1460,7 @@
   <dimension ref="B1:Z87"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1494,68 +1490,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:26" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
+      <c r="H1" s="122"/>
+      <c r="I1" s="122"/>
+      <c r="J1" s="122"/>
+      <c r="K1" s="122"/>
+      <c r="L1" s="122"/>
+      <c r="M1" s="122"/>
+      <c r="N1" s="122"/>
+      <c r="O1" s="122"/>
+      <c r="P1" s="122"/>
+      <c r="Q1" s="122"/>
+      <c r="R1" s="122"/>
+      <c r="S1" s="122"/>
+      <c r="T1" s="122"/>
+      <c r="U1" s="122"/>
+      <c r="V1" s="122"/>
+      <c r="W1" s="123"/>
+      <c r="X1" s="123"/>
+      <c r="Y1" s="123"/>
+      <c r="Z1" s="123"/>
     </row>
     <row r="2" spans="3:26" x14ac:dyDescent="0.35">
-      <c r="G2" s="79" t="s">
+      <c r="G2" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79"/>
-      <c r="J2" s="79"/>
-      <c r="K2" s="79"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="79"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="79"/>
-      <c r="R2" s="79"/>
-      <c r="S2" s="79"/>
-      <c r="T2" s="79"/>
-      <c r="U2" s="79"/>
-      <c r="V2" s="79"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="124"/>
+      <c r="M2" s="124"/>
+      <c r="N2" s="124"/>
+      <c r="O2" s="124"/>
+      <c r="P2" s="124"/>
+      <c r="Q2" s="124"/>
+      <c r="R2" s="124"/>
+      <c r="S2" s="124"/>
+      <c r="T2" s="124"/>
+      <c r="U2" s="124"/>
+      <c r="V2" s="124"/>
     </row>
     <row r="3" spans="3:26" x14ac:dyDescent="0.35">
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="80"/>
-      <c r="K3" s="80"/>
-      <c r="L3" s="80"/>
-      <c r="M3" s="80"/>
-      <c r="N3" s="80"/>
-      <c r="O3" s="80"/>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="80"/>
-      <c r="S3" s="80"/>
-      <c r="T3" s="80"/>
-      <c r="U3" s="80"/>
-      <c r="V3" s="80"/>
+      <c r="H3" s="125"/>
+      <c r="I3" s="125"/>
+      <c r="J3" s="125"/>
+      <c r="K3" s="125"/>
+      <c r="L3" s="125"/>
+      <c r="M3" s="125"/>
+      <c r="N3" s="125"/>
+      <c r="O3" s="125"/>
+      <c r="P3" s="125"/>
+      <c r="Q3" s="125"/>
+      <c r="R3" s="125"/>
+      <c r="S3" s="125"/>
+      <c r="T3" s="125"/>
+      <c r="U3" s="125"/>
+      <c r="V3" s="125"/>
       <c r="W3" s="1"/>
     </row>
     <row r="5" spans="3:26" ht="18" customHeight="1" x14ac:dyDescent="0.4">
@@ -1644,9 +1640,7 @@
         <v>4</v>
       </c>
       <c r="R7" s="8"/>
-      <c r="S7" s="35" t="s">
-        <v>10</v>
-      </c>
+      <c r="S7" s="35"/>
       <c r="T7" s="8"/>
       <c r="U7" s="5"/>
       <c r="V7" s="3"/>
@@ -1655,7 +1649,7 @@
     </row>
     <row r="8" spans="3:26" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1664,14 +1658,14 @@
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="8"/>
       <c r="K8" s="3"/>
       <c r="L8" s="7"/>
       <c r="N8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
@@ -1688,21 +1682,21 @@
     </row>
     <row r="9" spans="3:26" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
+      <c r="G9" s="126"/>
+      <c r="H9" s="126"/>
+      <c r="I9" s="126"/>
       <c r="J9" s="11"/>
       <c r="K9" s="3"/>
       <c r="L9" s="7"/>
       <c r="N9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
@@ -1719,7 +1713,7 @@
     </row>
     <row r="12" spans="3:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C12" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
@@ -1823,7 +1817,7 @@
     </row>
     <row r="16" spans="3:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C16" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D16" s="58"/>
       <c r="E16" s="54"/>
@@ -1833,7 +1827,7 @@
       <c r="I16" s="54"/>
       <c r="J16" s="54"/>
       <c r="K16" s="38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L16" s="53"/>
       <c r="M16" s="54"/>
@@ -1905,161 +1899,161 @@
     </row>
     <row r="20" spans="2:26" ht="22.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C20" s="22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="2:26" ht="1.5" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B22" s="108" t="s">
+      <c r="B22" s="85" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="86"/>
+      <c r="D22" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="109"/>
-      <c r="D22" s="116" t="s">
+      <c r="E22" s="93"/>
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="93"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="116"/>
-      <c r="F22" s="116"/>
-      <c r="G22" s="116"/>
-      <c r="H22" s="116"/>
-      <c r="I22" s="117"/>
-      <c r="J22" s="82" t="s">
+      <c r="K22" s="100"/>
+      <c r="L22" s="100"/>
+      <c r="M22" s="100"/>
+      <c r="N22" s="100"/>
+      <c r="O22" s="100"/>
+      <c r="P22" s="100"/>
+      <c r="Q22" s="100"/>
+      <c r="R22" s="100"/>
+      <c r="S22" s="100"/>
+      <c r="T22" s="101"/>
+      <c r="U22" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="83"/>
-      <c r="L22" s="83"/>
-      <c r="M22" s="83"/>
-      <c r="N22" s="83"/>
-      <c r="O22" s="83"/>
-      <c r="P22" s="83"/>
-      <c r="Q22" s="83"/>
-      <c r="R22" s="83"/>
-      <c r="S22" s="83"/>
-      <c r="T22" s="84"/>
-      <c r="U22" s="85" t="s">
+      <c r="V22" s="102"/>
+      <c r="W22" s="102"/>
+      <c r="X22" s="102"/>
+      <c r="Y22" s="102"/>
+      <c r="Z22" s="103"/>
+    </row>
+    <row r="23" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="87"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="95"/>
+      <c r="G23" s="95"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="V22" s="85"/>
-      <c r="W22" s="85"/>
-      <c r="X22" s="85"/>
-      <c r="Y22" s="85"/>
-      <c r="Z22" s="86"/>
-    </row>
-    <row r="23" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B23" s="110"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="118"/>
-      <c r="E23" s="118"/>
-      <c r="F23" s="118"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="118"/>
-      <c r="I23" s="119"/>
-      <c r="J23" s="82" t="s">
+      <c r="K23" s="100"/>
+      <c r="L23" s="100"/>
+      <c r="M23" s="100"/>
+      <c r="N23" s="101"/>
+      <c r="O23" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="K23" s="83"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="83"/>
-      <c r="N23" s="84"/>
-      <c r="O23" s="83" t="s">
+      <c r="P23" s="100"/>
+      <c r="Q23" s="100"/>
+      <c r="R23" s="100"/>
+      <c r="S23" s="100"/>
+      <c r="T23" s="101"/>
+      <c r="U23" s="104"/>
+      <c r="V23" s="104"/>
+      <c r="W23" s="104"/>
+      <c r="X23" s="104"/>
+      <c r="Y23" s="104"/>
+      <c r="Z23" s="105"/>
+    </row>
+    <row r="24" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="95"/>
+      <c r="G24" s="95"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="96"/>
+      <c r="J24" s="106" t="s">
         <v>25</v>
       </c>
-      <c r="P23" s="83"/>
-      <c r="Q23" s="83"/>
-      <c r="R23" s="83"/>
-      <c r="S23" s="83"/>
-      <c r="T23" s="84"/>
-      <c r="U23" s="87"/>
-      <c r="V23" s="87"/>
-      <c r="W23" s="87"/>
-      <c r="X23" s="87"/>
-      <c r="Y23" s="87"/>
-      <c r="Z23" s="88"/>
-    </row>
-    <row r="24" spans="2:26" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="110"/>
-      <c r="C24" s="111"/>
-      <c r="D24" s="118"/>
-      <c r="E24" s="118"/>
-      <c r="F24" s="118"/>
-      <c r="G24" s="118"/>
-      <c r="H24" s="118"/>
-      <c r="I24" s="119"/>
-      <c r="J24" s="89" t="s">
+      <c r="K24" s="107"/>
+      <c r="L24" s="107"/>
+      <c r="M24" s="108"/>
+      <c r="N24" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K24" s="90"/>
-      <c r="L24" s="90"/>
-      <c r="M24" s="91"/>
-      <c r="N24" s="24" t="s">
+      <c r="O24" s="106" t="s">
         <v>27</v>
       </c>
-      <c r="O24" s="89" t="s">
+      <c r="P24" s="107"/>
+      <c r="Q24" s="107"/>
+      <c r="R24" s="107"/>
+      <c r="S24" s="108"/>
+      <c r="T24" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="U24" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="P24" s="90"/>
-      <c r="Q24" s="90"/>
-      <c r="R24" s="90"/>
-      <c r="S24" s="91"/>
-      <c r="T24" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="U24" s="92" t="s">
+      <c r="V24" s="110"/>
+      <c r="W24" s="111"/>
+      <c r="X24" s="115" t="s">
         <v>29</v>
       </c>
-      <c r="V24" s="93"/>
-      <c r="W24" s="94"/>
-      <c r="X24" s="98" t="s">
+      <c r="Y24" s="115"/>
+      <c r="Z24" s="116"/>
+    </row>
+    <row r="25" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="89"/>
+      <c r="C25" s="90"/>
+      <c r="D25" s="97"/>
+      <c r="E25" s="97"/>
+      <c r="F25" s="97"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="98"/>
+      <c r="J25" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="Y24" s="98"/>
-      <c r="Z24" s="99"/>
-    </row>
-    <row r="25" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="112"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="120"/>
-      <c r="E25" s="120"/>
-      <c r="F25" s="120"/>
-      <c r="G25" s="120"/>
-      <c r="H25" s="120"/>
-      <c r="I25" s="121"/>
-      <c r="J25" s="102" t="s">
+      <c r="K25" s="120"/>
+      <c r="L25" s="120"/>
+      <c r="M25" s="121"/>
+      <c r="N25" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="K25" s="103"/>
-      <c r="L25" s="103"/>
-      <c r="M25" s="104"/>
-      <c r="N25" s="25" t="s">
+      <c r="O25" s="119" t="s">
+        <v>30</v>
+      </c>
+      <c r="P25" s="120"/>
+      <c r="Q25" s="120"/>
+      <c r="R25" s="120"/>
+      <c r="S25" s="121"/>
+      <c r="T25" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="O25" s="102" t="s">
-        <v>31</v>
-      </c>
-      <c r="P25" s="103"/>
-      <c r="Q25" s="103"/>
-      <c r="R25" s="103"/>
-      <c r="S25" s="104"/>
-      <c r="T25" s="26" t="s">
+      <c r="U25" s="112"/>
+      <c r="V25" s="113"/>
+      <c r="W25" s="114"/>
+      <c r="X25" s="117"/>
+      <c r="Y25" s="117"/>
+      <c r="Z25" s="118"/>
+    </row>
+    <row r="26" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="U25" s="95"/>
-      <c r="V25" s="96"/>
-      <c r="W25" s="97"/>
-      <c r="X25" s="100"/>
-      <c r="Y25" s="100"/>
-      <c r="Z25" s="101"/>
-    </row>
-    <row r="26" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" s="73"/>
-      <c r="D26" s="71"/>
-      <c r="E26" s="72"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="72"/>
-      <c r="H26" s="72"/>
-      <c r="I26" s="73"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="82"/>
+      <c r="F26" s="82"/>
+      <c r="G26" s="82"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="77"/>
       <c r="J26" s="40"/>
       <c r="K26" s="39"/>
       <c r="L26" s="39"/>
@@ -2079,14 +2073,14 @@
       <c r="Z26" s="41"/>
     </row>
     <row r="27" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="74"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="76"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="79"/>
+      <c r="D27" s="78"/>
+      <c r="E27" s="83"/>
+      <c r="F27" s="83"/>
+      <c r="G27" s="83"/>
+      <c r="H27" s="83"/>
+      <c r="I27" s="79"/>
       <c r="J27" s="42"/>
       <c r="K27" s="43"/>
       <c r="L27" s="43"/>
@@ -2106,14 +2100,14 @@
       <c r="Z27" s="45"/>
     </row>
     <row r="28" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="74"/>
-      <c r="C28" s="76"/>
-      <c r="D28" s="74"/>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75"/>
-      <c r="I28" s="76"/>
+      <c r="B28" s="78"/>
+      <c r="C28" s="79"/>
+      <c r="D28" s="78"/>
+      <c r="E28" s="83"/>
+      <c r="F28" s="83"/>
+      <c r="G28" s="83"/>
+      <c r="H28" s="83"/>
+      <c r="I28" s="79"/>
       <c r="J28" s="42"/>
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
@@ -2133,14 +2127,14 @@
       <c r="Z28" s="45"/>
     </row>
     <row r="29" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="74"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="74"/>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="76"/>
+      <c r="B29" s="78"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="78"/>
+      <c r="E29" s="83"/>
+      <c r="F29" s="83"/>
+      <c r="G29" s="83"/>
+      <c r="H29" s="83"/>
+      <c r="I29" s="79"/>
       <c r="J29" s="42"/>
       <c r="K29" s="43"/>
       <c r="L29" s="43"/>
@@ -2160,14 +2154,14 @@
       <c r="Z29" s="45"/>
     </row>
     <row r="30" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="74"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="76"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="78"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="83"/>
+      <c r="G30" s="83"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="79"/>
       <c r="J30" s="42"/>
       <c r="K30" s="43"/>
       <c r="L30" s="43"/>
@@ -2187,14 +2181,14 @@
       <c r="Z30" s="45"/>
     </row>
     <row r="31" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="74"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="74"/>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="75"/>
-      <c r="I31" s="76"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="79"/>
+      <c r="D31" s="78"/>
+      <c r="E31" s="83"/>
+      <c r="F31" s="83"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="79"/>
       <c r="J31" s="42"/>
       <c r="K31" s="43"/>
       <c r="L31" s="43"/>
@@ -2214,14 +2208,14 @@
       <c r="Z31" s="45"/>
     </row>
     <row r="32" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="74"/>
-      <c r="C32" s="76"/>
-      <c r="D32" s="74"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="76"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="79"/>
+      <c r="D32" s="78"/>
+      <c r="E32" s="83"/>
+      <c r="F32" s="83"/>
+      <c r="G32" s="83"/>
+      <c r="H32" s="83"/>
+      <c r="I32" s="79"/>
       <c r="J32" s="42"/>
       <c r="K32" s="43"/>
       <c r="L32" s="43"/>
@@ -2241,14 +2235,14 @@
       <c r="Z32" s="45"/>
     </row>
     <row r="33" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="74"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="74"/>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75"/>
-      <c r="I33" s="76"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="79"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="83"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="79"/>
       <c r="J33" s="42"/>
       <c r="K33" s="43"/>
       <c r="L33" s="43"/>
@@ -2268,14 +2262,14 @@
       <c r="Z33" s="45"/>
     </row>
     <row r="34" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="74"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="75"/>
-      <c r="I34" s="76"/>
+      <c r="B34" s="78"/>
+      <c r="C34" s="79"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="83"/>
+      <c r="F34" s="83"/>
+      <c r="G34" s="83"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="79"/>
       <c r="J34" s="42"/>
       <c r="K34" s="43"/>
       <c r="L34" s="43"/>
@@ -2295,14 +2289,14 @@
       <c r="Z34" s="45"/>
     </row>
     <row r="35" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="114"/>
-      <c r="C35" s="115"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="76"/>
+      <c r="B35" s="91"/>
+      <c r="C35" s="92"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="79"/>
       <c r="J35" s="46"/>
       <c r="K35" s="43"/>
       <c r="L35" s="43"/>
@@ -2322,16 +2316,16 @@
       <c r="Z35" s="45"/>
     </row>
     <row r="36" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="71" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="73"/>
-      <c r="D36" s="71"/>
-      <c r="E36" s="72"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="73"/>
+      <c r="B36" s="76" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="77"/>
+      <c r="D36" s="76"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="77"/>
       <c r="J36" s="40"/>
       <c r="K36" s="39"/>
       <c r="L36" s="39"/>
@@ -2351,14 +2345,14 @@
       <c r="Z36" s="41"/>
     </row>
     <row r="37" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="74"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="76"/>
+      <c r="B37" s="78"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="78"/>
+      <c r="E37" s="83"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="79"/>
       <c r="J37" s="42"/>
       <c r="K37" s="43"/>
       <c r="L37" s="43"/>
@@ -2378,14 +2372,14 @@
       <c r="Z37" s="45"/>
     </row>
     <row r="38" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="74"/>
-      <c r="C38" s="76"/>
-      <c r="D38" s="74"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="75"/>
-      <c r="I38" s="76"/>
+      <c r="B38" s="78"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="83"/>
+      <c r="F38" s="83"/>
+      <c r="G38" s="83"/>
+      <c r="H38" s="83"/>
+      <c r="I38" s="79"/>
       <c r="J38" s="42"/>
       <c r="K38" s="43"/>
       <c r="L38" s="43"/>
@@ -2405,14 +2399,14 @@
       <c r="Z38" s="45"/>
     </row>
     <row r="39" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="74"/>
-      <c r="C39" s="76"/>
-      <c r="D39" s="74"/>
-      <c r="E39" s="75"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="75"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="76"/>
+      <c r="B39" s="78"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="78"/>
+      <c r="E39" s="83"/>
+      <c r="F39" s="83"/>
+      <c r="G39" s="83"/>
+      <c r="H39" s="83"/>
+      <c r="I39" s="79"/>
       <c r="J39" s="42"/>
       <c r="K39" s="43"/>
       <c r="L39" s="43"/>
@@ -2432,14 +2426,14 @@
       <c r="Z39" s="45"/>
     </row>
     <row r="40" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="74"/>
-      <c r="C40" s="76"/>
-      <c r="D40" s="74"/>
-      <c r="E40" s="75"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="75"/>
-      <c r="I40" s="76"/>
+      <c r="B40" s="78"/>
+      <c r="C40" s="79"/>
+      <c r="D40" s="78"/>
+      <c r="E40" s="83"/>
+      <c r="F40" s="83"/>
+      <c r="G40" s="83"/>
+      <c r="H40" s="83"/>
+      <c r="I40" s="79"/>
       <c r="J40" s="42"/>
       <c r="K40" s="43"/>
       <c r="L40" s="43"/>
@@ -2459,14 +2453,14 @@
       <c r="Z40" s="45"/>
     </row>
     <row r="41" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="74"/>
-      <c r="C41" s="76"/>
-      <c r="D41" s="74"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="76"/>
+      <c r="B41" s="78"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="78"/>
+      <c r="E41" s="83"/>
+      <c r="F41" s="83"/>
+      <c r="G41" s="83"/>
+      <c r="H41" s="83"/>
+      <c r="I41" s="79"/>
       <c r="J41" s="42"/>
       <c r="K41" s="43"/>
       <c r="L41" s="43"/>
@@ -2486,14 +2480,14 @@
       <c r="Z41" s="45"/>
     </row>
     <row r="42" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="74"/>
-      <c r="C42" s="76"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="75"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="75"/>
-      <c r="H42" s="75"/>
-      <c r="I42" s="76"/>
+      <c r="B42" s="78"/>
+      <c r="C42" s="79"/>
+      <c r="D42" s="78"/>
+      <c r="E42" s="83"/>
+      <c r="F42" s="83"/>
+      <c r="G42" s="83"/>
+      <c r="H42" s="83"/>
+      <c r="I42" s="79"/>
       <c r="J42" s="42"/>
       <c r="K42" s="43"/>
       <c r="L42" s="43"/>
@@ -2513,14 +2507,14 @@
       <c r="Z42" s="45"/>
     </row>
     <row r="43" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="74"/>
-      <c r="C43" s="76"/>
-      <c r="D43" s="74"/>
-      <c r="E43" s="75"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="75"/>
-      <c r="H43" s="75"/>
-      <c r="I43" s="76"/>
+      <c r="B43" s="78"/>
+      <c r="C43" s="79"/>
+      <c r="D43" s="78"/>
+      <c r="E43" s="83"/>
+      <c r="F43" s="83"/>
+      <c r="G43" s="83"/>
+      <c r="H43" s="83"/>
+      <c r="I43" s="79"/>
       <c r="J43" s="42"/>
       <c r="K43" s="43"/>
       <c r="L43" s="43"/>
@@ -2540,14 +2534,14 @@
       <c r="Z43" s="45"/>
     </row>
     <row r="44" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="74"/>
-      <c r="C44" s="76"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="75"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="75"/>
-      <c r="H44" s="75"/>
-      <c r="I44" s="76"/>
+      <c r="B44" s="78"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="83"/>
+      <c r="F44" s="83"/>
+      <c r="G44" s="83"/>
+      <c r="H44" s="83"/>
+      <c r="I44" s="79"/>
       <c r="J44" s="42"/>
       <c r="K44" s="43"/>
       <c r="L44" s="43"/>
@@ -2567,14 +2561,14 @@
       <c r="Z44" s="45"/>
     </row>
     <row r="45" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="114"/>
-      <c r="C45" s="115"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="75"/>
-      <c r="I45" s="76"/>
+      <c r="B45" s="91"/>
+      <c r="C45" s="92"/>
+      <c r="D45" s="78"/>
+      <c r="E45" s="83"/>
+      <c r="F45" s="83"/>
+      <c r="G45" s="83"/>
+      <c r="H45" s="83"/>
+      <c r="I45" s="79"/>
       <c r="J45" s="46"/>
       <c r="K45" s="43"/>
       <c r="L45" s="43"/>
@@ -2594,16 +2588,16 @@
       <c r="Z45" s="45"/>
     </row>
     <row r="46" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="71" t="s">
-        <v>38</v>
-      </c>
-      <c r="C46" s="73"/>
-      <c r="D46" s="71"/>
-      <c r="E46" s="72"/>
-      <c r="F46" s="72"/>
-      <c r="G46" s="72"/>
-      <c r="H46" s="72"/>
-      <c r="I46" s="73"/>
+      <c r="B46" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="C46" s="77"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="82"/>
+      <c r="H46" s="82"/>
+      <c r="I46" s="77"/>
       <c r="J46" s="40"/>
       <c r="K46" s="39"/>
       <c r="L46" s="39"/>
@@ -2623,14 +2617,14 @@
       <c r="Z46" s="41"/>
     </row>
     <row r="47" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="74"/>
-      <c r="C47" s="76"/>
-      <c r="D47" s="74"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="75"/>
-      <c r="I47" s="76"/>
+      <c r="B47" s="78"/>
+      <c r="C47" s="79"/>
+      <c r="D47" s="78"/>
+      <c r="E47" s="83"/>
+      <c r="F47" s="83"/>
+      <c r="G47" s="83"/>
+      <c r="H47" s="83"/>
+      <c r="I47" s="79"/>
       <c r="J47" s="42"/>
       <c r="K47" s="43"/>
       <c r="L47" s="43"/>
@@ -2650,14 +2644,14 @@
       <c r="Z47" s="45"/>
     </row>
     <row r="48" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="74"/>
-      <c r="C48" s="76"/>
-      <c r="D48" s="74"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="75"/>
-      <c r="G48" s="75"/>
-      <c r="H48" s="75"/>
-      <c r="I48" s="76"/>
+      <c r="B48" s="78"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="78"/>
+      <c r="E48" s="83"/>
+      <c r="F48" s="83"/>
+      <c r="G48" s="83"/>
+      <c r="H48" s="83"/>
+      <c r="I48" s="79"/>
       <c r="J48" s="42"/>
       <c r="K48" s="43"/>
       <c r="L48" s="43"/>
@@ -2677,14 +2671,14 @@
       <c r="Z48" s="45"/>
     </row>
     <row r="49" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="74"/>
-      <c r="C49" s="76"/>
-      <c r="D49" s="74"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="75"/>
-      <c r="I49" s="76"/>
+      <c r="B49" s="78"/>
+      <c r="C49" s="79"/>
+      <c r="D49" s="78"/>
+      <c r="E49" s="83"/>
+      <c r="F49" s="83"/>
+      <c r="G49" s="83"/>
+      <c r="H49" s="83"/>
+      <c r="I49" s="79"/>
       <c r="J49" s="42"/>
       <c r="K49" s="43"/>
       <c r="L49" s="43"/>
@@ -2704,14 +2698,14 @@
       <c r="Z49" s="45"/>
     </row>
     <row r="50" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="74"/>
-      <c r="C50" s="76"/>
-      <c r="D50" s="74"/>
-      <c r="E50" s="75"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="75"/>
-      <c r="H50" s="75"/>
-      <c r="I50" s="76"/>
+      <c r="B50" s="78"/>
+      <c r="C50" s="79"/>
+      <c r="D50" s="78"/>
+      <c r="E50" s="83"/>
+      <c r="F50" s="83"/>
+      <c r="G50" s="83"/>
+      <c r="H50" s="83"/>
+      <c r="I50" s="79"/>
       <c r="J50" s="42"/>
       <c r="K50" s="43"/>
       <c r="L50" s="43"/>
@@ -2731,14 +2725,14 @@
       <c r="Z50" s="45"/>
     </row>
     <row r="51" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="74"/>
-      <c r="C51" s="76"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="75"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="75"/>
-      <c r="H51" s="75"/>
-      <c r="I51" s="76"/>
+      <c r="B51" s="78"/>
+      <c r="C51" s="79"/>
+      <c r="D51" s="78"/>
+      <c r="E51" s="83"/>
+      <c r="F51" s="83"/>
+      <c r="G51" s="83"/>
+      <c r="H51" s="83"/>
+      <c r="I51" s="79"/>
       <c r="J51" s="42"/>
       <c r="K51" s="43"/>
       <c r="L51" s="43"/>
@@ -2758,14 +2752,14 @@
       <c r="Z51" s="45"/>
     </row>
     <row r="52" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="74"/>
-      <c r="C52" s="76"/>
-      <c r="D52" s="74"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="75"/>
-      <c r="I52" s="76"/>
+      <c r="B52" s="78"/>
+      <c r="C52" s="79"/>
+      <c r="D52" s="78"/>
+      <c r="E52" s="83"/>
+      <c r="F52" s="83"/>
+      <c r="G52" s="83"/>
+      <c r="H52" s="83"/>
+      <c r="I52" s="79"/>
       <c r="J52" s="42"/>
       <c r="K52" s="43"/>
       <c r="L52" s="43"/>
@@ -2785,14 +2779,14 @@
       <c r="Z52" s="45"/>
     </row>
     <row r="53" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="74"/>
-      <c r="C53" s="76"/>
-      <c r="D53" s="74"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="75"/>
-      <c r="H53" s="75"/>
-      <c r="I53" s="76"/>
+      <c r="B53" s="78"/>
+      <c r="C53" s="79"/>
+      <c r="D53" s="78"/>
+      <c r="E53" s="83"/>
+      <c r="F53" s="83"/>
+      <c r="G53" s="83"/>
+      <c r="H53" s="83"/>
+      <c r="I53" s="79"/>
       <c r="J53" s="42"/>
       <c r="K53" s="43"/>
       <c r="L53" s="43"/>
@@ -2812,14 +2806,14 @@
       <c r="Z53" s="45"/>
     </row>
     <row r="54" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="74"/>
-      <c r="C54" s="76"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="75"/>
-      <c r="F54" s="75"/>
-      <c r="G54" s="75"/>
-      <c r="H54" s="75"/>
-      <c r="I54" s="76"/>
+      <c r="B54" s="78"/>
+      <c r="C54" s="79"/>
+      <c r="D54" s="78"/>
+      <c r="E54" s="83"/>
+      <c r="F54" s="83"/>
+      <c r="G54" s="83"/>
+      <c r="H54" s="83"/>
+      <c r="I54" s="79"/>
       <c r="J54" s="42"/>
       <c r="K54" s="43"/>
       <c r="L54" s="43"/>
@@ -2839,14 +2833,14 @@
       <c r="Z54" s="45"/>
     </row>
     <row r="55" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="114"/>
-      <c r="C55" s="115"/>
-      <c r="D55" s="74"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="75"/>
-      <c r="I55" s="76"/>
+      <c r="B55" s="91"/>
+      <c r="C55" s="92"/>
+      <c r="D55" s="78"/>
+      <c r="E55" s="83"/>
+      <c r="F55" s="83"/>
+      <c r="G55" s="83"/>
+      <c r="H55" s="83"/>
+      <c r="I55" s="79"/>
       <c r="J55" s="46"/>
       <c r="K55" s="43"/>
       <c r="L55" s="43"/>
@@ -2866,16 +2860,16 @@
       <c r="Z55" s="45"/>
     </row>
     <row r="56" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B56" s="71" t="s">
-        <v>39</v>
-      </c>
-      <c r="C56" s="73"/>
-      <c r="D56" s="71"/>
-      <c r="E56" s="72"/>
-      <c r="F56" s="72"/>
-      <c r="G56" s="72"/>
-      <c r="H56" s="72"/>
-      <c r="I56" s="73"/>
+      <c r="B56" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="77"/>
+      <c r="D56" s="76"/>
+      <c r="E56" s="82"/>
+      <c r="F56" s="82"/>
+      <c r="G56" s="82"/>
+      <c r="H56" s="82"/>
+      <c r="I56" s="77"/>
       <c r="J56" s="40"/>
       <c r="K56" s="39"/>
       <c r="L56" s="39"/>
@@ -2895,14 +2889,14 @@
       <c r="Z56" s="41"/>
     </row>
     <row r="57" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="74"/>
-      <c r="C57" s="76"/>
-      <c r="D57" s="74"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="75"/>
-      <c r="I57" s="76"/>
+      <c r="B57" s="78"/>
+      <c r="C57" s="79"/>
+      <c r="D57" s="78"/>
+      <c r="E57" s="83"/>
+      <c r="F57" s="83"/>
+      <c r="G57" s="83"/>
+      <c r="H57" s="83"/>
+      <c r="I57" s="79"/>
       <c r="J57" s="42"/>
       <c r="K57" s="43"/>
       <c r="L57" s="43"/>
@@ -2922,14 +2916,14 @@
       <c r="Z57" s="45"/>
     </row>
     <row r="58" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="74"/>
-      <c r="C58" s="76"/>
-      <c r="D58" s="74"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="75"/>
-      <c r="I58" s="76"/>
+      <c r="B58" s="78"/>
+      <c r="C58" s="79"/>
+      <c r="D58" s="78"/>
+      <c r="E58" s="83"/>
+      <c r="F58" s="83"/>
+      <c r="G58" s="83"/>
+      <c r="H58" s="83"/>
+      <c r="I58" s="79"/>
       <c r="J58" s="42"/>
       <c r="K58" s="43"/>
       <c r="L58" s="43"/>
@@ -2949,14 +2943,14 @@
       <c r="Z58" s="45"/>
     </row>
     <row r="59" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="74"/>
-      <c r="C59" s="76"/>
-      <c r="D59" s="74"/>
-      <c r="E59" s="75"/>
-      <c r="F59" s="75"/>
-      <c r="G59" s="75"/>
-      <c r="H59" s="75"/>
-      <c r="I59" s="76"/>
+      <c r="B59" s="78"/>
+      <c r="C59" s="79"/>
+      <c r="D59" s="78"/>
+      <c r="E59" s="83"/>
+      <c r="F59" s="83"/>
+      <c r="G59" s="83"/>
+      <c r="H59" s="83"/>
+      <c r="I59" s="79"/>
       <c r="J59" s="42"/>
       <c r="K59" s="43"/>
       <c r="L59" s="43"/>
@@ -2976,14 +2970,14 @@
       <c r="Z59" s="45"/>
     </row>
     <row r="60" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="74"/>
-      <c r="C60" s="76"/>
-      <c r="D60" s="74"/>
-      <c r="E60" s="75"/>
-      <c r="F60" s="75"/>
-      <c r="G60" s="75"/>
-      <c r="H60" s="75"/>
-      <c r="I60" s="76"/>
+      <c r="B60" s="78"/>
+      <c r="C60" s="79"/>
+      <c r="D60" s="78"/>
+      <c r="E60" s="83"/>
+      <c r="F60" s="83"/>
+      <c r="G60" s="83"/>
+      <c r="H60" s="83"/>
+      <c r="I60" s="79"/>
       <c r="J60" s="42"/>
       <c r="K60" s="43"/>
       <c r="L60" s="43"/>
@@ -3003,14 +2997,14 @@
       <c r="Z60" s="45"/>
     </row>
     <row r="61" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="74"/>
-      <c r="C61" s="76"/>
-      <c r="D61" s="74"/>
-      <c r="E61" s="75"/>
-      <c r="F61" s="75"/>
-      <c r="G61" s="75"/>
-      <c r="H61" s="75"/>
-      <c r="I61" s="76"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="79"/>
+      <c r="D61" s="78"/>
+      <c r="E61" s="83"/>
+      <c r="F61" s="83"/>
+      <c r="G61" s="83"/>
+      <c r="H61" s="83"/>
+      <c r="I61" s="79"/>
       <c r="J61" s="42"/>
       <c r="K61" s="43"/>
       <c r="L61" s="43"/>
@@ -3030,14 +3024,14 @@
       <c r="Z61" s="45"/>
     </row>
     <row r="62" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B62" s="74"/>
-      <c r="C62" s="76"/>
-      <c r="D62" s="74"/>
-      <c r="E62" s="75"/>
-      <c r="F62" s="75"/>
-      <c r="G62" s="75"/>
-      <c r="H62" s="75"/>
-      <c r="I62" s="76"/>
+      <c r="B62" s="78"/>
+      <c r="C62" s="79"/>
+      <c r="D62" s="78"/>
+      <c r="E62" s="83"/>
+      <c r="F62" s="83"/>
+      <c r="G62" s="83"/>
+      <c r="H62" s="83"/>
+      <c r="I62" s="79"/>
       <c r="J62" s="42"/>
       <c r="K62" s="43"/>
       <c r="L62" s="43"/>
@@ -3057,14 +3051,14 @@
       <c r="Z62" s="45"/>
     </row>
     <row r="63" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="74"/>
-      <c r="C63" s="76"/>
-      <c r="D63" s="74"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="75"/>
-      <c r="I63" s="76"/>
+      <c r="B63" s="78"/>
+      <c r="C63" s="79"/>
+      <c r="D63" s="78"/>
+      <c r="E63" s="83"/>
+      <c r="F63" s="83"/>
+      <c r="G63" s="83"/>
+      <c r="H63" s="83"/>
+      <c r="I63" s="79"/>
       <c r="J63" s="42"/>
       <c r="K63" s="43"/>
       <c r="L63" s="43"/>
@@ -3084,14 +3078,14 @@
       <c r="Z63" s="45"/>
     </row>
     <row r="64" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B64" s="74"/>
-      <c r="C64" s="76"/>
-      <c r="D64" s="74"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="75"/>
-      <c r="H64" s="75"/>
-      <c r="I64" s="76"/>
+      <c r="B64" s="78"/>
+      <c r="C64" s="79"/>
+      <c r="D64" s="78"/>
+      <c r="E64" s="83"/>
+      <c r="F64" s="83"/>
+      <c r="G64" s="83"/>
+      <c r="H64" s="83"/>
+      <c r="I64" s="79"/>
       <c r="J64" s="42"/>
       <c r="K64" s="43"/>
       <c r="L64" s="43"/>
@@ -3111,14 +3105,14 @@
       <c r="Z64" s="45"/>
     </row>
     <row r="65" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="114"/>
-      <c r="C65" s="115"/>
-      <c r="D65" s="74"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="75"/>
-      <c r="H65" s="75"/>
-      <c r="I65" s="76"/>
+      <c r="B65" s="91"/>
+      <c r="C65" s="92"/>
+      <c r="D65" s="78"/>
+      <c r="E65" s="83"/>
+      <c r="F65" s="83"/>
+      <c r="G65" s="83"/>
+      <c r="H65" s="83"/>
+      <c r="I65" s="79"/>
       <c r="J65" s="46"/>
       <c r="K65" s="43"/>
       <c r="L65" s="43"/>
@@ -3138,16 +3132,16 @@
       <c r="Z65" s="45"/>
     </row>
     <row r="66" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="C66" s="73"/>
-      <c r="D66" s="71"/>
-      <c r="E66" s="72"/>
-      <c r="F66" s="72"/>
-      <c r="G66" s="72"/>
-      <c r="H66" s="72"/>
-      <c r="I66" s="73"/>
+      <c r="B66" s="76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C66" s="77"/>
+      <c r="D66" s="76"/>
+      <c r="E66" s="82"/>
+      <c r="F66" s="82"/>
+      <c r="G66" s="82"/>
+      <c r="H66" s="82"/>
+      <c r="I66" s="77"/>
       <c r="J66" s="40"/>
       <c r="K66" s="39"/>
       <c r="L66" s="39"/>
@@ -3167,14 +3161,14 @@
       <c r="Z66" s="41"/>
     </row>
     <row r="67" spans="2:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="74"/>
-      <c r="C67" s="76"/>
-      <c r="D67" s="74"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="75"/>
-      <c r="H67" s="75"/>
-      <c r="I67" s="76"/>
+      <c r="B67" s="78"/>
+      <c r="C67" s="79"/>
+      <c r="D67" s="78"/>
+      <c r="E67" s="83"/>
+      <c r="F67" s="83"/>
+      <c r="G67" s="83"/>
+      <c r="H67" s="83"/>
+      <c r="I67" s="79"/>
       <c r="J67" s="42"/>
       <c r="K67" s="43"/>
       <c r="L67" s="43"/>
@@ -3194,14 +3188,14 @@
       <c r="Z67" s="45"/>
     </row>
     <row r="68" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B68" s="74"/>
-      <c r="C68" s="76"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
-      <c r="I68" s="76"/>
+      <c r="B68" s="78"/>
+      <c r="C68" s="79"/>
+      <c r="D68" s="78"/>
+      <c r="E68" s="83"/>
+      <c r="F68" s="83"/>
+      <c r="G68" s="83"/>
+      <c r="H68" s="83"/>
+      <c r="I68" s="79"/>
       <c r="J68" s="42"/>
       <c r="K68" s="43"/>
       <c r="L68" s="43"/>
@@ -3221,14 +3215,14 @@
       <c r="Z68" s="45"/>
     </row>
     <row r="69" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B69" s="74"/>
-      <c r="C69" s="76"/>
-      <c r="D69" s="74"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="75"/>
-      <c r="H69" s="75"/>
-      <c r="I69" s="76"/>
+      <c r="B69" s="78"/>
+      <c r="C69" s="79"/>
+      <c r="D69" s="78"/>
+      <c r="E69" s="83"/>
+      <c r="F69" s="83"/>
+      <c r="G69" s="83"/>
+      <c r="H69" s="83"/>
+      <c r="I69" s="79"/>
       <c r="J69" s="42"/>
       <c r="K69" s="43"/>
       <c r="L69" s="43"/>
@@ -3248,14 +3242,14 @@
       <c r="Z69" s="45"/>
     </row>
     <row r="70" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="74"/>
-      <c r="C70" s="76"/>
-      <c r="D70" s="74"/>
-      <c r="E70" s="75"/>
-      <c r="F70" s="75"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="75"/>
-      <c r="I70" s="76"/>
+      <c r="B70" s="78"/>
+      <c r="C70" s="79"/>
+      <c r="D70" s="78"/>
+      <c r="E70" s="83"/>
+      <c r="F70" s="83"/>
+      <c r="G70" s="83"/>
+      <c r="H70" s="83"/>
+      <c r="I70" s="79"/>
       <c r="J70" s="42"/>
       <c r="K70" s="43"/>
       <c r="L70" s="43"/>
@@ -3275,14 +3269,14 @@
       <c r="Z70" s="45"/>
     </row>
     <row r="71" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="74"/>
-      <c r="C71" s="76"/>
-      <c r="D71" s="74"/>
-      <c r="E71" s="75"/>
-      <c r="F71" s="75"/>
-      <c r="G71" s="75"/>
-      <c r="H71" s="75"/>
-      <c r="I71" s="76"/>
+      <c r="B71" s="78"/>
+      <c r="C71" s="79"/>
+      <c r="D71" s="78"/>
+      <c r="E71" s="83"/>
+      <c r="F71" s="83"/>
+      <c r="G71" s="83"/>
+      <c r="H71" s="83"/>
+      <c r="I71" s="79"/>
       <c r="J71" s="42"/>
       <c r="K71" s="43"/>
       <c r="L71" s="43"/>
@@ -3302,14 +3296,14 @@
       <c r="Z71" s="45"/>
     </row>
     <row r="72" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B72" s="74"/>
-      <c r="C72" s="76"/>
-      <c r="D72" s="74"/>
-      <c r="E72" s="75"/>
-      <c r="F72" s="75"/>
-      <c r="G72" s="75"/>
-      <c r="H72" s="75"/>
-      <c r="I72" s="76"/>
+      <c r="B72" s="78"/>
+      <c r="C72" s="79"/>
+      <c r="D72" s="78"/>
+      <c r="E72" s="83"/>
+      <c r="F72" s="83"/>
+      <c r="G72" s="83"/>
+      <c r="H72" s="83"/>
+      <c r="I72" s="79"/>
       <c r="J72" s="42"/>
       <c r="K72" s="43"/>
       <c r="L72" s="43"/>
@@ -3329,14 +3323,14 @@
       <c r="Z72" s="45"/>
     </row>
     <row r="73" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B73" s="74"/>
-      <c r="C73" s="76"/>
-      <c r="D73" s="74"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="75"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
-      <c r="I73" s="76"/>
+      <c r="B73" s="78"/>
+      <c r="C73" s="79"/>
+      <c r="D73" s="78"/>
+      <c r="E73" s="83"/>
+      <c r="F73" s="83"/>
+      <c r="G73" s="83"/>
+      <c r="H73" s="83"/>
+      <c r="I73" s="79"/>
       <c r="J73" s="42"/>
       <c r="K73" s="43"/>
       <c r="L73" s="43"/>
@@ -3356,14 +3350,14 @@
       <c r="Z73" s="45"/>
     </row>
     <row r="74" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="74"/>
-      <c r="C74" s="76"/>
-      <c r="D74" s="74"/>
-      <c r="E74" s="75"/>
-      <c r="F74" s="75"/>
-      <c r="G74" s="75"/>
-      <c r="H74" s="75"/>
-      <c r="I74" s="76"/>
+      <c r="B74" s="78"/>
+      <c r="C74" s="79"/>
+      <c r="D74" s="78"/>
+      <c r="E74" s="83"/>
+      <c r="F74" s="83"/>
+      <c r="G74" s="83"/>
+      <c r="H74" s="83"/>
+      <c r="I74" s="79"/>
       <c r="J74" s="42"/>
       <c r="K74" s="43"/>
       <c r="L74" s="43"/>
@@ -3383,14 +3377,14 @@
       <c r="Z74" s="45"/>
     </row>
     <row r="75" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B75" s="105"/>
-      <c r="C75" s="106"/>
-      <c r="D75" s="105"/>
-      <c r="E75" s="107"/>
-      <c r="F75" s="107"/>
-      <c r="G75" s="107"/>
-      <c r="H75" s="107"/>
-      <c r="I75" s="106"/>
+      <c r="B75" s="80"/>
+      <c r="C75" s="81"/>
+      <c r="D75" s="80"/>
+      <c r="E75" s="84"/>
+      <c r="F75" s="84"/>
+      <c r="G75" s="84"/>
+      <c r="H75" s="84"/>
+      <c r="I75" s="81"/>
       <c r="J75" s="47"/>
       <c r="K75" s="48"/>
       <c r="L75" s="48"/>
@@ -3421,7 +3415,7 @@
     <row r="78" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B78" s="23"/>
       <c r="C78" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D78" s="14"/>
       <c r="E78" s="14"/>
@@ -3435,15 +3429,15 @@
       <c r="M78" s="15"/>
       <c r="N78" s="16"/>
       <c r="O78" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="P78" s="28"/>
-      <c r="Q78" s="67"/>
-      <c r="R78" s="67"/>
+      <c r="Q78" s="127"/>
+      <c r="R78" s="127"/>
       <c r="S78" s="28"/>
       <c r="T78" s="29"/>
       <c r="U78" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V78" s="28"/>
       <c r="W78" s="28"/>
@@ -3455,52 +3449,43 @@
       <c r="B79" s="16"/>
       <c r="M79" s="17"/>
       <c r="N79" s="16"/>
-      <c r="O79" s="122"/>
-      <c r="P79" s="123"/>
-      <c r="Q79" s="123"/>
-      <c r="R79" s="123"/>
-      <c r="S79" s="123"/>
-      <c r="T79" s="123"/>
+      <c r="O79" s="67"/>
+      <c r="P79" s="68"/>
+      <c r="Q79" s="68"/>
+      <c r="R79" s="68"/>
+      <c r="S79" s="68"/>
+      <c r="T79" s="68"/>
       <c r="U79" s="30"/>
-      <c r="V79" s="123"/>
-      <c r="W79" s="123"/>
-      <c r="X79" s="123"/>
-      <c r="Y79" s="123"/>
-      <c r="Z79" s="127"/>
+      <c r="V79" s="68"/>
+      <c r="W79" s="68"/>
+      <c r="X79" s="68"/>
+      <c r="Y79" s="68"/>
+      <c r="Z79" s="71"/>
     </row>
     <row r="80" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B80" s="16"/>
       <c r="M80" s="17"/>
       <c r="N80" s="16"/>
-      <c r="O80" s="124"/>
-      <c r="P80" s="125"/>
-      <c r="Q80" s="125"/>
-      <c r="R80" s="125"/>
-      <c r="S80" s="125"/>
-      <c r="T80" s="125"/>
-      <c r="U80" s="130"/>
-      <c r="V80" s="125"/>
-      <c r="W80" s="125"/>
-      <c r="X80" s="125"/>
-      <c r="Y80" s="125"/>
-      <c r="Z80" s="128"/>
+      <c r="O80" s="69"/>
+      <c r="P80" s="70"/>
+      <c r="Q80" s="70"/>
+      <c r="R80" s="70"/>
+      <c r="S80" s="70"/>
+      <c r="T80" s="70"/>
+      <c r="U80" s="74"/>
+      <c r="V80" s="70"/>
+      <c r="W80" s="70"/>
+      <c r="X80" s="70"/>
+      <c r="Y80" s="70"/>
+      <c r="Z80" s="72"/>
     </row>
     <row r="81" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B81" s="16"/>
       <c r="M81" s="17"/>
       <c r="N81" s="16"/>
-      <c r="O81" s="124"/>
-      <c r="P81" s="126"/>
-      <c r="Q81" s="126"/>
-      <c r="R81" s="126"/>
-      <c r="S81" s="126"/>
-      <c r="T81" s="126"/>
-      <c r="U81" s="124"/>
-      <c r="V81" s="126"/>
-      <c r="W81" s="126"/>
-      <c r="X81" s="126"/>
-      <c r="Y81" s="126"/>
-      <c r="Z81" s="129"/>
+      <c r="O81" s="69"/>
+      <c r="U81" s="69"/>
+      <c r="Z81" s="73"/>
     </row>
     <row r="82" spans="2:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B82" s="18"/>
@@ -3516,60 +3501,24 @@
       <c r="L82" s="19"/>
       <c r="M82" s="20"/>
       <c r="N82" s="16"/>
-      <c r="O82" s="124"/>
-      <c r="P82" s="126"/>
-      <c r="Q82" s="126"/>
-      <c r="R82" s="126"/>
-      <c r="S82" s="126"/>
-      <c r="T82" s="126"/>
-      <c r="U82" s="124"/>
-      <c r="V82" s="126"/>
-      <c r="W82" s="126"/>
-      <c r="X82" s="126"/>
-      <c r="Y82" s="126"/>
-      <c r="Z82" s="129"/>
+      <c r="O82" s="69"/>
+      <c r="U82" s="69"/>
+      <c r="Z82" s="73"/>
     </row>
     <row r="83" spans="2:26" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="O83" s="124"/>
-      <c r="P83" s="126"/>
-      <c r="Q83" s="126"/>
-      <c r="R83" s="126"/>
-      <c r="S83" s="126"/>
-      <c r="T83" s="126"/>
-      <c r="U83" s="124"/>
-      <c r="V83" s="126"/>
-      <c r="W83" s="126"/>
-      <c r="X83" s="126"/>
-      <c r="Y83" s="126"/>
-      <c r="Z83" s="129"/>
+      <c r="O83" s="69"/>
+      <c r="U83" s="69"/>
+      <c r="Z83" s="73"/>
     </row>
     <row r="84" spans="2:26" x14ac:dyDescent="0.35">
-      <c r="O84" s="124"/>
-      <c r="P84" s="126"/>
-      <c r="Q84" s="126"/>
-      <c r="R84" s="126"/>
-      <c r="S84" s="126"/>
-      <c r="T84" s="126"/>
-      <c r="U84" s="124"/>
-      <c r="V84" s="126"/>
-      <c r="W84" s="126"/>
-      <c r="X84" s="126"/>
-      <c r="Y84" s="126"/>
-      <c r="Z84" s="129"/>
+      <c r="O84" s="69"/>
+      <c r="U84" s="69"/>
+      <c r="Z84" s="73"/>
     </row>
     <row r="85" spans="2:26" x14ac:dyDescent="0.35">
-      <c r="O85" s="124"/>
-      <c r="P85" s="126"/>
-      <c r="Q85" s="126"/>
-      <c r="R85" s="126"/>
-      <c r="S85" s="126"/>
-      <c r="T85" s="126"/>
-      <c r="U85" s="124"/>
-      <c r="V85" s="126"/>
-      <c r="W85" s="126"/>
-      <c r="X85" s="126"/>
-      <c r="Y85" s="126"/>
-      <c r="Z85" s="129"/>
+      <c r="O85" s="69"/>
+      <c r="U85" s="69"/>
+      <c r="Z85" s="73"/>
     </row>
     <row r="86" spans="2:26" x14ac:dyDescent="0.35">
       <c r="O86" s="16"/>
@@ -3578,7 +3527,7 @@
       <c r="R86" s="31"/>
       <c r="S86" s="31"/>
       <c r="T86" s="31"/>
-      <c r="U86" s="131"/>
+      <c r="U86" s="75"/>
       <c r="V86" s="31"/>
       <c r="W86" s="31"/>
       <c r="X86" s="31"/>
@@ -3586,30 +3535,32 @@
       <c r="Z86" s="32"/>
     </row>
     <row r="87" spans="2:26" ht="16" x14ac:dyDescent="0.4">
-      <c r="O87" s="68"/>
-      <c r="P87" s="69"/>
-      <c r="Q87" s="69"/>
-      <c r="R87" s="69"/>
-      <c r="S87" s="69"/>
-      <c r="T87" s="70"/>
-      <c r="U87" s="132"/>
-      <c r="V87" s="133"/>
-      <c r="W87" s="133"/>
-      <c r="X87" s="133"/>
-      <c r="Y87" s="133"/>
-      <c r="Z87" s="134"/>
+      <c r="O87" s="128"/>
+      <c r="P87" s="129"/>
+      <c r="Q87" s="129"/>
+      <c r="R87" s="129"/>
+      <c r="S87" s="129"/>
+      <c r="T87" s="130"/>
+      <c r="U87" s="131"/>
+      <c r="V87" s="132"/>
+      <c r="W87" s="132"/>
+      <c r="X87" s="132"/>
+      <c r="Y87" s="132"/>
+      <c r="Z87" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B66:C75"/>
-    <mergeCell ref="D66:I75"/>
-    <mergeCell ref="B22:C25"/>
-    <mergeCell ref="B26:C35"/>
-    <mergeCell ref="B36:C45"/>
-    <mergeCell ref="B46:C55"/>
-    <mergeCell ref="B56:C65"/>
-    <mergeCell ref="D56:I65"/>
-    <mergeCell ref="D22:I25"/>
+    <mergeCell ref="U87:Z87"/>
+    <mergeCell ref="Q78:R78"/>
+    <mergeCell ref="O87:T87"/>
+    <mergeCell ref="D26:I35"/>
+    <mergeCell ref="D36:I45"/>
+    <mergeCell ref="D46:I55"/>
+    <mergeCell ref="G1:V1"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="G2:V2"/>
+    <mergeCell ref="G3:V3"/>
+    <mergeCell ref="G9:I9"/>
     <mergeCell ref="J22:T22"/>
     <mergeCell ref="U22:Z23"/>
     <mergeCell ref="J23:N23"/>
@@ -3620,17 +3571,15 @@
     <mergeCell ref="X24:Z25"/>
     <mergeCell ref="J25:M25"/>
     <mergeCell ref="O25:S25"/>
-    <mergeCell ref="G1:V1"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="G2:V2"/>
-    <mergeCell ref="G3:V3"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="Q78:R78"/>
-    <mergeCell ref="O87:T87"/>
-    <mergeCell ref="D26:I35"/>
-    <mergeCell ref="D36:I45"/>
-    <mergeCell ref="D46:I55"/>
-    <mergeCell ref="U87:Z87"/>
+    <mergeCell ref="B66:C75"/>
+    <mergeCell ref="D66:I75"/>
+    <mergeCell ref="B22:C25"/>
+    <mergeCell ref="B26:C35"/>
+    <mergeCell ref="B36:C45"/>
+    <mergeCell ref="B46:C55"/>
+    <mergeCell ref="B56:C65"/>
+    <mergeCell ref="D56:I65"/>
+    <mergeCell ref="D22:I25"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: Update performance data sorting and adjust image height in export functionality
</commit_message>
<xml_diff>
--- a/public/assets/file/Template_ICP.xlsx
+++ b/public/assets/file/Template_ICP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\core\public\assets\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD60CE94-AE85-42AC-B74C-D7D5B0EE355F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1D25B1-C7CD-4F9C-95C6-F790E43F8C3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1049,6 +1049,15 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1059,15 +1068,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1460,7 +1460,7 @@
   <dimension ref="B1:Z87"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1477,15 +1477,12 @@
     <col min="12" max="12" width="7.36328125" customWidth="1"/>
     <col min="13" max="13" width="6.6328125" customWidth="1"/>
     <col min="14" max="14" width="28.6328125" customWidth="1"/>
-    <col min="15" max="15" width="4.08984375" customWidth="1"/>
+    <col min="15" max="15" width="6.6328125" customWidth="1"/>
     <col min="17" max="17" width="5.6328125" customWidth="1"/>
     <col min="18" max="18" width="11.54296875" customWidth="1"/>
     <col min="19" max="19" width="9.08984375" customWidth="1"/>
     <col min="20" max="20" width="29.36328125" customWidth="1"/>
-    <col min="21" max="22" width="6.6328125" customWidth="1"/>
-    <col min="23" max="23" width="7.6328125" customWidth="1"/>
-    <col min="24" max="24" width="6.6328125" customWidth="1"/>
-    <col min="26" max="26" width="6.6328125" customWidth="1"/>
+    <col min="21" max="26" width="10.6328125" customWidth="1"/>
     <col min="27" max="27" width="4.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3432,8 +3429,8 @@
         <v>35</v>
       </c>
       <c r="P78" s="28"/>
-      <c r="Q78" s="127"/>
-      <c r="R78" s="127"/>
+      <c r="Q78" s="130"/>
+      <c r="R78" s="130"/>
       <c r="S78" s="28"/>
       <c r="T78" s="29"/>
       <c r="U78" s="2" t="s">
@@ -3535,18 +3532,18 @@
       <c r="Z86" s="32"/>
     </row>
     <row r="87" spans="2:26" ht="16" x14ac:dyDescent="0.4">
-      <c r="O87" s="128"/>
-      <c r="P87" s="129"/>
-      <c r="Q87" s="129"/>
-      <c r="R87" s="129"/>
-      <c r="S87" s="129"/>
-      <c r="T87" s="130"/>
-      <c r="U87" s="131"/>
-      <c r="V87" s="132"/>
-      <c r="W87" s="132"/>
-      <c r="X87" s="132"/>
-      <c r="Y87" s="132"/>
-      <c r="Z87" s="133"/>
+      <c r="O87" s="131"/>
+      <c r="P87" s="132"/>
+      <c r="Q87" s="132"/>
+      <c r="R87" s="132"/>
+      <c r="S87" s="132"/>
+      <c r="T87" s="133"/>
+      <c r="U87" s="127"/>
+      <c r="V87" s="128"/>
+      <c r="W87" s="128"/>
+      <c r="X87" s="128"/>
+      <c r="Y87" s="128"/>
+      <c r="Z87" s="129"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -3582,7 +3579,8 @@
     <mergeCell ref="D22:I25"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>